<commit_message>
Fix hierarchical metrics wrongly computed
</commit_message>
<xml_diff>
--- a/benchmark/results/hierarchical_metrics/sp_rdp_its.100.xlsx
+++ b/benchmark/results/hierarchical_metrics/sp_rdp_its.100.xlsx
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.9999911990424558</v>
       </c>
       <c r="C2" t="n">
         <v>0.9840904993690284</v>
@@ -567,7 +567,7 @@
         <v>0.9999555100769676</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9968220244418458</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
         <v>1</v>
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.9999911990424558</v>
       </c>
       <c r="C3" t="n">
         <v>0.971437469413178</v>
@@ -637,7 +637,7 @@
         <v>0.9999555100769676</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9935934510833296</v>
+        <v>0.9967611336032388</v>
       </c>
       <c r="H3" t="n">
         <v>0.9967611336032388</v>
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8571428571428571</v>
+        <v>0.9999911990424558</v>
       </c>
       <c r="C4" t="n">
         <v>0.9777230493675138</v>
@@ -707,7 +707,7 @@
         <v>0.9999555100769676</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9952051192927106</v>
+        <v>0.9983779399837792</v>
       </c>
       <c r="H4" t="n">
         <v>0.9983779399837792</v>

</xml_diff>